<commit_message>
correct status detail weight, hba1c, med_diabetes
</commit_message>
<xml_diff>
--- a/data_processing_elements-LOF.xlsx
+++ b/data_processing_elements-LOF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7589CCA4-0814-4405-A820-9731A4167695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C905E2-F622-4ED7-A96C-7E4121E29432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -2253,10 +2253,10 @@
   <dimension ref="A1:W84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S9" sqref="S9"/>
+      <selection pane="bottomRight" activeCell="O57" sqref="O57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3135,7 +3135,7 @@
         <v>25</v>
       </c>
       <c r="Q18" s="12" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="R18" s="12" t="s">
         <v>200</v>
@@ -3741,7 +3741,7 @@
         <v>25</v>
       </c>
       <c r="Q31" s="12" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="R31" s="12" t="s">
         <v>45</v>
@@ -4918,8 +4918,8 @@
       <c r="P57" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="Q57" s="15" t="s">
-        <v>26</v>
+      <c r="Q57" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="R57" s="15" t="s">
         <v>200</v>

</xml_diff>

<commit_message>
correct valuetype vegetable and fruit quantity
</commit_message>
<xml_diff>
--- a/data_processing_elements-LOF.xlsx
+++ b/data_processing_elements-LOF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbtiali\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C905E2-F622-4ED7-A96C-7E4121E29432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF09DD3-41A9-4A38-8D02-F169BED83064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
+    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{36FA7FB5-5526-4959-8292-475F227215C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data_processing_elements" sheetId="8" r:id="rId1"/>
@@ -2253,10 +2253,10 @@
   <dimension ref="A1:W84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O57" sqref="O57"/>
+      <selection pane="bottomRight" activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4050,7 +4050,7 @@
         <v>147</v>
       </c>
       <c r="F38" s="12" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="G38" s="12" t="s">
         <v>148</v>
@@ -4128,7 +4128,7 @@
         <v>155</v>
       </c>
       <c r="F40" s="12" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="G40" s="12" t="s">
         <v>148</v>

</xml_diff>